<commit_message>
Add quaternion functions (#149)
* add quaternion multiplication function

* add quat transform function

* add quat to body axes function

* add vector by quaternion rotation function

* add quat2rv function

* add rv2quat function and update tests

* use scipy to make life easier

* small bugfix in qtrans.m (qmag update)

* update functions/tests and add quat <-> dcm conversion functions

* add quat <-> euler transformation functions

* add quat <-> eigen transformation functions

* add dcm <-> euler transformation functions

* add invalid test cases for quat to eigen transformation

* add vec rotation by dcm function + matlab bugfix

* update sheet
</commit_message>
<xml_diff>
--- a/Astro Software.xlsx
+++ b/Astro Software.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2853" uniqueCount="1497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2899" uniqueCount="1537">
   <si>
     <t xml:space="preserve">Astrodynamics Software </t>
   </si>
@@ -4654,6 +4654,96 @@
     <t xml:space="preserve">valladopy.mathtime.julian_date.convtime</t>
   </si>
   <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.quat_multiply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qtimesq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.quat_transform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qtrans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.quat2body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q2body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.vec_by_quat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qtrvec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.vec_by_dcm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcmtrvec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.quat2rv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q2rv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.rv2quat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rv2q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.quat2dcm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q2dcm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.dcm2quat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcm2q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.quat2euler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q2euler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.euler2quat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">euler2q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.quat2eigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q2eigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.eigen2quat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eigen2q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.dcm2euler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcm2euler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.rotations.euler2dcm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">euler2dcm</t>
+  </si>
+  <si>
     <t xml:space="preserve">valladopy.mathtime.utils.hms2sec</t>
   </si>
   <si>
@@ -4703,6 +4793,36 @@
   </si>
   <si>
     <t xml:space="preserve">valladopy.mathtime.utils.jd2sse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.vector.rot1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.vector.rot2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.vector.rot3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.vector.rot1mat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.vector.rot2mat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.vector.rot3mat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.vector.angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">angl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valladopy.mathtime.vector.unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
   </si>
   <si>
     <t xml:space="preserve">valladopy.constants</t>
@@ -4858,15 +4978,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -5002,7 +5122,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5203,11 +5323,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5217,6 +5333,18 @@
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -5474,9 +5602,9 @@
   <dimension ref="A1:P349"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="7" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="7" topLeftCell="A343" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="O233" activeCellId="0" sqref="O233"/>
+      <selection pane="bottomLeft" activeCell="H353" activeCellId="0" sqref="H353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="11.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10395,7 +10523,8 @@
         <v>459</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="1"/>
       <c r="B261" s="10" t="s">
         <v>3</v>
       </c>
@@ -10411,6 +10540,8 @@
       <c r="F261" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="G261" s="2"/>
+      <c r="H261" s="2"/>
       <c r="I261" s="2" t="n">
         <v>311</v>
       </c>
@@ -10420,9 +10551,13 @@
       <c r="K261" s="2" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="262" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="1"/>
+      <c r="L261" s="2"/>
+      <c r="M261" s="2"/>
+      <c r="N261" s="2"/>
+      <c r="O261" s="2"/>
+      <c r="P261" s="2"/>
+    </row>
+    <row r="262" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="10" t="s">
         <v>3</v>
       </c>
@@ -10438,8 +10573,6 @@
       <c r="F262" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G262" s="2"/>
-      <c r="H262" s="2"/>
       <c r="I262" s="2" t="n">
         <v>310</v>
       </c>
@@ -10449,11 +10582,6 @@
       <c r="K262" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="L262" s="2"/>
-      <c r="M262" s="2"/>
-      <c r="N262" s="2"/>
-      <c r="O262" s="2"/>
-      <c r="P262" s="2"/>
     </row>
     <row r="263" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C263" s="1" t="s">
@@ -10602,45 +10730,45 @@
         <v>473</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="1"/>
       <c r="B273" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="C273" s="1"/>
       <c r="D273" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="E273" s="1"/>
       <c r="F273" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="G273" s="2"/>
+      <c r="H273" s="2"/>
+      <c r="I273" s="2"/>
       <c r="J273" s="2" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="274" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="1"/>
+      <c r="K273" s="2"/>
+      <c r="L273" s="2"/>
+      <c r="M273" s="2"/>
+      <c r="N273" s="2"/>
+      <c r="O273" s="2"/>
+      <c r="P273" s="2"/>
+    </row>
+    <row r="274" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C274" s="1"/>
       <c r="D274" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E274" s="1"/>
       <c r="F274" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G274" s="2"/>
-      <c r="H274" s="2"/>
-      <c r="I274" s="2"/>
       <c r="J274" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="K274" s="2"/>
-      <c r="L274" s="2"/>
-      <c r="M274" s="2"/>
-      <c r="N274" s="2"/>
-      <c r="O274" s="2"/>
-      <c r="P274" s="2"/>
     </row>
     <row r="275" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="276" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10955,7 +11083,7 @@
       <c r="N289" s="14"/>
       <c r="O289" s="14"/>
     </row>
-    <row r="290" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="9" t="s">
         <v>3</v>
       </c>
@@ -10974,31 +11102,22 @@
       <c r="F290" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="G290" s="2"/>
+      <c r="H290" s="2"/>
+      <c r="I290" s="2"/>
       <c r="J290" s="2" t="s">
         <v>498</v>
       </c>
       <c r="K290" s="2" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="291" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="1"/>
-      <c r="B291" s="1"/>
-      <c r="C291" s="1"/>
-      <c r="D291" s="1"/>
-      <c r="E291" s="1"/>
-      <c r="F291" s="2"/>
-      <c r="G291" s="2"/>
-      <c r="H291" s="2"/>
-      <c r="I291" s="2"/>
-      <c r="J291" s="2"/>
-      <c r="K291" s="2"/>
-      <c r="L291" s="2"/>
-      <c r="M291" s="2"/>
-      <c r="N291" s="2"/>
-      <c r="O291" s="2"/>
-      <c r="P291" s="2"/>
-    </row>
+      <c r="L290" s="2"/>
+      <c r="M290" s="2"/>
+      <c r="N290" s="2"/>
+      <c r="O290" s="2"/>
+      <c r="P290" s="2"/>
+    </row>
+    <row r="291" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="292" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="7" t="s">
         <v>3</v>
@@ -11787,38 +11906,33 @@
         <v>567</v>
       </c>
     </row>
-    <row r="339" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="1"/>
       <c r="B339" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="C339" s="1"/>
+      <c r="D339" s="1"/>
       <c r="E339" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F339" s="2"/>
+      <c r="G339" s="2"/>
+      <c r="H339" s="2"/>
+      <c r="I339" s="2"/>
       <c r="J339" s="2" t="s">
         <v>568</v>
       </c>
       <c r="K339" s="2" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="340" s="13" customFormat="true" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A340" s="1"/>
-      <c r="B340" s="1"/>
-      <c r="C340" s="1"/>
-      <c r="D340" s="1"/>
-      <c r="E340" s="1"/>
-      <c r="F340" s="2"/>
-      <c r="G340" s="2"/>
-      <c r="H340" s="2"/>
-      <c r="I340" s="2"/>
-      <c r="J340" s="2"/>
-      <c r="K340" s="2"/>
-      <c r="L340" s="2"/>
-      <c r="M340" s="2"/>
-      <c r="N340" s="2"/>
-      <c r="O340" s="2"/>
-      <c r="P340" s="2"/>
-    </row>
+      <c r="L339" s="2"/>
+      <c r="M339" s="2"/>
+      <c r="N339" s="2"/>
+      <c r="O339" s="2"/>
+      <c r="P339" s="2"/>
+    </row>
+    <row r="340" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="341" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="342" customFormat="false" ht="11.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="343" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14749,21 +14863,21 @@
       </c>
     </row>
     <row r="67" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0"/>
+      <c r="A67" s="24"/>
       <c r="B67" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="C67" s="0"/>
-      <c r="D67" s="0"/>
-      <c r="E67" s="0"/>
-      <c r="F67" s="0"/>
-      <c r="G67" s="0"/>
-      <c r="H67" s="0"/>
-      <c r="I67" s="0"/>
-      <c r="J67" s="0"/>
-      <c r="K67" s="0"/>
-      <c r="L67" s="0"/>
-      <c r="M67" s="0"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="24"/>
+      <c r="J67" s="24"/>
+      <c r="K67" s="24"/>
+      <c r="L67" s="24"/>
+      <c r="M67" s="24"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="24" t="s">
@@ -15653,20 +15767,20 @@
         <v>454</v>
       </c>
     </row>
-    <row r="221" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="0"/>
-      <c r="B221" s="0"/>
-      <c r="C221" s="0"/>
-      <c r="D221" s="0"/>
-      <c r="E221" s="0"/>
-      <c r="F221" s="0"/>
-      <c r="G221" s="0"/>
-      <c r="H221" s="0"/>
-      <c r="I221" s="0"/>
-      <c r="J221" s="0"/>
-      <c r="K221" s="0"/>
-      <c r="L221" s="0"/>
-      <c r="M221" s="0"/>
+    <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="24"/>
+      <c r="B221" s="24"/>
+      <c r="C221" s="24"/>
+      <c r="D221" s="24"/>
+      <c r="E221" s="24"/>
+      <c r="F221" s="24"/>
+      <c r="G221" s="24"/>
+      <c r="H221" s="24"/>
+      <c r="I221" s="24"/>
+      <c r="J221" s="24"/>
+      <c r="K221" s="24"/>
+      <c r="L221" s="24"/>
+      <c r="M221" s="24"/>
     </row>
     <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="36"/>
@@ -15857,27 +15971,39 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="24" t="s">
         <v>1060</v>
       </c>
-    </row>
-    <row r="257" s="36" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B256" s="0"/>
+      <c r="C256" s="0"/>
+      <c r="D256" s="0"/>
+      <c r="E256" s="0"/>
+      <c r="F256" s="0"/>
+      <c r="G256" s="0"/>
+      <c r="H256" s="0"/>
+      <c r="I256" s="0"/>
+      <c r="J256" s="0"/>
+      <c r="K256" s="0"/>
+      <c r="L256" s="0"/>
+      <c r="M256" s="0"/>
+    </row>
+    <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="24" t="s">
         <v>1061</v>
       </c>
-      <c r="B257" s="0"/>
-      <c r="C257" s="0"/>
-      <c r="D257" s="0"/>
-      <c r="E257" s="0"/>
-      <c r="F257" s="0"/>
-      <c r="G257" s="0"/>
-      <c r="H257" s="0"/>
-      <c r="I257" s="0"/>
-      <c r="J257" s="0"/>
-      <c r="K257" s="0"/>
-      <c r="L257" s="0"/>
-      <c r="M257" s="0"/>
+      <c r="B257" s="24"/>
+      <c r="C257" s="24"/>
+      <c r="D257" s="24"/>
+      <c r="E257" s="24"/>
+      <c r="F257" s="24"/>
+      <c r="G257" s="24"/>
+      <c r="H257" s="24"/>
+      <c r="I257" s="24"/>
+      <c r="J257" s="24"/>
+      <c r="K257" s="24"/>
+      <c r="L257" s="24"/>
+      <c r="M257" s="24"/>
     </row>
     <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="36"/>
@@ -16334,10 +16460,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB1049"/>
+  <dimension ref="A1:AB1072"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C211" activeCellId="0" sqref="C211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16930,7 +17056,7 @@
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="41"/>
       <c r="B52" s="41"/>
-      <c r="C52" s="49" t="s">
+      <c r="C52" s="43" t="s">
         <v>1244</v>
       </c>
       <c r="D52" s="44" t="s">
@@ -16980,7 +17106,7 @@
       <c r="D56" s="44" t="s">
         <v>1250</v>
       </c>
-      <c r="E56" s="50" t="s">
+      <c r="E56" s="49" t="s">
         <v>1251</v>
       </c>
     </row>
@@ -16993,7 +17119,7 @@
       <c r="D57" s="46" t="s">
         <v>1253</v>
       </c>
-      <c r="E57" s="51" t="s">
+      <c r="E57" s="50" t="s">
         <v>1251</v>
       </c>
     </row>
@@ -17172,10 +17298,10 @@
       <c r="C72" s="43" t="s">
         <v>1272</v>
       </c>
-      <c r="D72" s="52" t="s">
+      <c r="D72" s="51" t="s">
         <v>1273</v>
       </c>
-      <c r="E72" s="53" t="s">
+      <c r="E72" s="52" t="s">
         <v>1274</v>
       </c>
     </row>
@@ -17185,8 +17311,8 @@
       <c r="C73" s="43" t="s">
         <v>1275</v>
       </c>
-      <c r="D73" s="52"/>
-      <c r="E73" s="52"/>
+      <c r="D73" s="51"/>
+      <c r="E73" s="51"/>
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="41"/>
@@ -17194,8 +17320,8 @@
       <c r="C74" s="43" t="s">
         <v>1276</v>
       </c>
-      <c r="D74" s="52"/>
-      <c r="E74" s="52"/>
+      <c r="D74" s="51"/>
+      <c r="E74" s="51"/>
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="41"/>
@@ -17203,10 +17329,10 @@
       <c r="C75" s="43" t="s">
         <v>1277</v>
       </c>
-      <c r="D75" s="52" t="s">
+      <c r="D75" s="51" t="s">
         <v>1278</v>
       </c>
-      <c r="E75" s="53" t="s">
+      <c r="E75" s="52" t="s">
         <v>1274</v>
       </c>
     </row>
@@ -17216,8 +17342,8 @@
       <c r="C76" s="43" t="s">
         <v>1279</v>
       </c>
-      <c r="D76" s="52"/>
-      <c r="E76" s="52"/>
+      <c r="D76" s="51"/>
+      <c r="E76" s="51"/>
     </row>
     <row r="77" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="41"/>
@@ -17225,8 +17351,8 @@
       <c r="C77" s="43" t="s">
         <v>1280</v>
       </c>
-      <c r="D77" s="52"/>
-      <c r="E77" s="52"/>
+      <c r="D77" s="51"/>
+      <c r="E77" s="51"/>
     </row>
     <row r="78" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="41"/>
@@ -17234,8 +17360,8 @@
       <c r="C78" s="43" t="s">
         <v>1281</v>
       </c>
-      <c r="D78" s="52"/>
-      <c r="E78" s="52"/>
+      <c r="D78" s="51"/>
+      <c r="E78" s="51"/>
     </row>
     <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="41"/>
@@ -18004,7 +18130,7 @@
       <c r="D152" s="44" t="s">
         <v>1405</v>
       </c>
-      <c r="E152" s="50" t="s">
+      <c r="E152" s="49" t="s">
         <v>1406</v>
       </c>
     </row>
@@ -18017,7 +18143,7 @@
       <c r="D153" s="44" t="s">
         <v>1408</v>
       </c>
-      <c r="E153" s="50" t="s">
+      <c r="E153" s="49" t="s">
         <v>1406</v>
       </c>
     </row>
@@ -18060,7 +18186,7 @@
       <c r="D157" s="44" t="s">
         <v>1416</v>
       </c>
-      <c r="E157" s="50" t="s">
+      <c r="E157" s="49" t="s">
         <v>1417</v>
       </c>
     </row>
@@ -18466,7 +18592,7 @@
     <row r="197" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="41"/>
       <c r="B197" s="41"/>
-      <c r="C197" s="43" t="s">
+      <c r="C197" s="53" t="s">
         <v>1478</v>
       </c>
       <c r="D197" s="44" t="s">
@@ -18476,7 +18602,7 @@
     <row r="198" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="41"/>
       <c r="B198" s="41"/>
-      <c r="C198" s="43" t="s">
+      <c r="C198" s="53" t="s">
         <v>1480</v>
       </c>
       <c r="D198" s="44" t="s">
@@ -18486,7 +18612,7 @@
     <row r="199" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="41"/>
       <c r="B199" s="41"/>
-      <c r="C199" s="43" t="s">
+      <c r="C199" s="53" t="s">
         <v>1482</v>
       </c>
       <c r="D199" s="44" t="s">
@@ -18496,7 +18622,7 @@
     <row r="200" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="41"/>
       <c r="B200" s="41"/>
-      <c r="C200" s="43" t="s">
+      <c r="C200" s="53" t="s">
         <v>1484</v>
       </c>
       <c r="D200" s="44" t="s">
@@ -18506,7 +18632,7 @@
     <row r="201" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="41"/>
       <c r="B201" s="41"/>
-      <c r="C201" s="43" t="s">
+      <c r="C201" s="53" t="s">
         <v>1486</v>
       </c>
       <c r="D201" s="44" t="s">
@@ -18516,7 +18642,7 @@
     <row r="202" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="41"/>
       <c r="B202" s="41"/>
-      <c r="C202" s="43" t="s">
+      <c r="C202" s="53" t="s">
         <v>1488</v>
       </c>
       <c r="D202" s="44" t="s">
@@ -18526,7 +18652,7 @@
     <row r="203" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="41"/>
       <c r="B203" s="41"/>
-      <c r="C203" s="43" t="s">
+      <c r="C203" s="53" t="s">
         <v>1490</v>
       </c>
       <c r="D203" s="44" t="s">
@@ -18536,7 +18662,7 @@
     <row r="204" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="41"/>
       <c r="B204" s="41"/>
-      <c r="C204" s="43" t="s">
+      <c r="C204" s="53" t="s">
         <v>1492</v>
       </c>
       <c r="D204" s="44" t="s">
@@ -18546,105 +18672,266 @@
     <row r="205" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="41"/>
       <c r="B205" s="41"/>
-      <c r="C205" s="45" t="s">
+      <c r="C205" s="53" t="s">
         <v>1494</v>
       </c>
-      <c r="D205" s="46" t="s">
+      <c r="D205" s="44" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="41"/>
+      <c r="B206" s="41"/>
+      <c r="C206" s="53" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D206" s="44" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="41"/>
+      <c r="B207" s="41"/>
+      <c r="C207" s="53" t="s">
+        <v>1498</v>
+      </c>
+      <c r="D207" s="44" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="41"/>
+      <c r="B208" s="41"/>
+      <c r="C208" s="53" t="s">
+        <v>1500</v>
+      </c>
+      <c r="D208" s="44" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="41"/>
+      <c r="B209" s="41"/>
+      <c r="C209" s="53" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D209" s="44" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="41"/>
+      <c r="B210" s="41"/>
+      <c r="C210" s="53" t="s">
+        <v>1504</v>
+      </c>
+      <c r="D210" s="54" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="41"/>
+      <c r="B211" s="41"/>
+      <c r="C211" s="53" t="s">
+        <v>1506</v>
+      </c>
+      <c r="D211" s="54" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="41"/>
+      <c r="B212" s="41"/>
+      <c r="C212" s="43" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D212" s="44" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="41"/>
+      <c r="B213" s="41"/>
+      <c r="C213" s="43" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D213" s="44" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="41"/>
+      <c r="B214" s="41"/>
+      <c r="C214" s="43" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D214" s="44" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="41"/>
+      <c r="B215" s="41"/>
+      <c r="C215" s="43" t="s">
+        <v>1514</v>
+      </c>
+      <c r="D215" s="44" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="41"/>
+      <c r="B216" s="41"/>
+      <c r="C216" s="43" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D216" s="44" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="41"/>
+      <c r="B217" s="41"/>
+      <c r="C217" s="43" t="s">
+        <v>1518</v>
+      </c>
+      <c r="D217" s="44" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="41"/>
+      <c r="B218" s="41"/>
+      <c r="C218" s="43" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D218" s="44" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="41"/>
+      <c r="B219" s="41"/>
+      <c r="C219" s="43" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D219" s="44" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="41"/>
+      <c r="B220" s="41"/>
+      <c r="C220" s="53" t="s">
+        <v>1524</v>
+      </c>
+      <c r="D220" s="54" t="s">
         <v>210</v>
       </c>
-      <c r="E205" s="45"/>
-    </row>
-    <row r="206" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="52" t="s">
+    </row>
+    <row r="221" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="41"/>
+      <c r="B221" s="41"/>
+      <c r="C221" s="53" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D221" s="44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="41"/>
+      <c r="B222" s="41"/>
+      <c r="C222" s="53" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D222" s="44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="41"/>
+      <c r="B223" s="41"/>
+      <c r="C223" s="53" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D223" s="44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="41"/>
+      <c r="B224" s="41"/>
+      <c r="C224" s="53" t="s">
+        <v>1528</v>
+      </c>
+      <c r="D224" s="44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="41"/>
+      <c r="B225" s="41"/>
+      <c r="C225" s="53" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D225" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="41"/>
+      <c r="B226" s="41"/>
+      <c r="C226" s="53" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D226" s="44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="41"/>
+      <c r="B227" s="41"/>
+      <c r="C227" s="53" t="s">
+        <v>1531</v>
+      </c>
+      <c r="D227" s="44" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="41"/>
+      <c r="B228" s="41"/>
+      <c r="C228" s="55" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D228" s="46" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E228" s="45"/>
+    </row>
+    <row r="229" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="51" t="s">
         <v>1416</v>
       </c>
-      <c r="B206" s="52"/>
-      <c r="C206" s="53" t="s">
-        <v>1495</v>
-      </c>
-      <c r="D206" s="44" t="s">
+      <c r="B229" s="51"/>
+      <c r="C229" s="52" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D229" s="44" t="s">
         <v>572</v>
       </c>
-      <c r="E206" s="43" t="s">
-        <v>1496</v>
-      </c>
-    </row>
-    <row r="207" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="52"/>
-      <c r="B207" s="52"/>
-      <c r="C207" s="53"/>
-      <c r="D207" s="44" t="s">
+      <c r="E229" s="43" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="51"/>
+      <c r="B230" s="51"/>
+      <c r="C230" s="52"/>
+      <c r="D230" s="44" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="208" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D208" s="44"/>
-    </row>
-    <row r="209" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D209" s="44"/>
-    </row>
-    <row r="210" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D210" s="44"/>
-    </row>
-    <row r="211" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D211" s="44"/>
-    </row>
-    <row r="212" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D212" s="44"/>
-    </row>
-    <row r="213" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D213" s="44"/>
-    </row>
-    <row r="214" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D214" s="44"/>
-    </row>
-    <row r="215" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D215" s="44"/>
-    </row>
-    <row r="216" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D216" s="44"/>
-    </row>
-    <row r="217" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D217" s="44"/>
-    </row>
-    <row r="218" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D218" s="44"/>
-    </row>
-    <row r="219" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D219" s="44"/>
-    </row>
-    <row r="220" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D220" s="44"/>
-    </row>
-    <row r="221" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D221" s="44"/>
-    </row>
-    <row r="222" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D222" s="44"/>
-    </row>
-    <row r="223" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D223" s="44"/>
-    </row>
-    <row r="224" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D224" s="44"/>
-    </row>
-    <row r="225" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D225" s="44"/>
-    </row>
-    <row r="226" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D226" s="44"/>
-    </row>
-    <row r="227" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D227" s="44"/>
-    </row>
-    <row r="228" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D228" s="44"/>
-    </row>
-    <row r="229" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D229" s="44"/>
-    </row>
-    <row r="230" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D230" s="44"/>
     </row>
     <row r="231" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D231" s="44"/>
@@ -21102,6 +21389,75 @@
     </row>
     <row r="1049" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1049" s="44"/>
+    </row>
+    <row r="1050" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1050" s="44"/>
+    </row>
+    <row r="1051" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1051" s="44"/>
+    </row>
+    <row r="1052" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1052" s="44"/>
+    </row>
+    <row r="1053" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1053" s="44"/>
+    </row>
+    <row r="1054" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1054" s="44"/>
+    </row>
+    <row r="1055" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1055" s="44"/>
+    </row>
+    <row r="1056" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1056" s="44"/>
+    </row>
+    <row r="1057" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1057" s="44"/>
+    </row>
+    <row r="1058" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1058" s="44"/>
+    </row>
+    <row r="1059" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1059" s="44"/>
+    </row>
+    <row r="1060" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1060" s="44"/>
+    </row>
+    <row r="1061" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1061" s="44"/>
+    </row>
+    <row r="1062" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1062" s="44"/>
+    </row>
+    <row r="1063" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1063" s="44"/>
+    </row>
+    <row r="1064" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1064" s="44"/>
+    </row>
+    <row r="1065" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1065" s="44"/>
+    </row>
+    <row r="1066" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1066" s="44"/>
+    </row>
+    <row r="1067" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1067" s="44"/>
+    </row>
+    <row r="1068" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1068" s="44"/>
+    </row>
+    <row r="1069" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1069" s="44"/>
+    </row>
+    <row r="1070" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1070" s="44"/>
+    </row>
+    <row r="1071" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1071" s="44"/>
+    </row>
+    <row r="1072" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1072" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -21119,9 +21475,9 @@
     <mergeCell ref="D75:D78"/>
     <mergeCell ref="E75:E78"/>
     <mergeCell ref="B125:B185"/>
-    <mergeCell ref="A186:B205"/>
-    <mergeCell ref="A206:B207"/>
-    <mergeCell ref="C206:C207"/>
+    <mergeCell ref="A186:B228"/>
+    <mergeCell ref="A229:B230"/>
+    <mergeCell ref="C229:C230"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>